<commit_message>
Made all student IDs unique in the Excel hsheets
</commit_message>
<xml_diff>
--- a/data/mentors.xlsx
+++ b/data/mentors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisarojas/GDrive/Graduate/Winter2018/CSCI5020G_Collaborative_Design_and_Research/project/repo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D631F8C9-BDA6-DC47-8678-1DDFA20EB1EA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B0C0F4-5C00-BA4D-9C04-23EC6270A06F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="460" windowWidth="14560" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1824,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90549B2-1AA3-BE46-90D8-E7C8AB09A7F5}">
   <dimension ref="A1:AF943"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D70" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="2" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>100123456</v>
+        <v>100000941</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>115</v>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="3" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>100123456</v>
+        <v>100000942</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>122</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="4" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>100123456</v>
+        <v>100000943</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>127</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="5" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>100123456</v>
+        <v>100000944</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>131</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="6" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>100123456</v>
+        <v>100000945</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>120</v>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="7" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>100123456</v>
+        <v>100000946</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>139</v>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="8" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>100123456</v>
+        <v>100000947</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>142</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="9" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>100123456</v>
+        <v>100000948</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>145</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="10" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>100123456</v>
+        <v>100000949</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>148</v>
@@ -2833,7 +2833,7 @@
     </row>
     <row r="11" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>100123456</v>
+        <v>100000950</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>153</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="12" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>100123456</v>
+        <v>100000951</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>157</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="13" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>100123456</v>
+        <v>100000952</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>161</v>
@@ -3127,7 +3127,7 @@
     </row>
     <row r="14" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>100123456</v>
+        <v>100000953</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>165</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="15" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>100123456</v>
+        <v>100000954</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>129</v>
@@ -3323,7 +3323,7 @@
     </row>
     <row r="16" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>100123456</v>
+        <v>100000955</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>170</v>
@@ -3421,7 +3421,7 @@
     </row>
     <row r="17" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>100123456</v>
+        <v>100000956</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>172</v>
@@ -3519,7 +3519,7 @@
     </row>
     <row r="18" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>100123456</v>
+        <v>100000957</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>175</v>
@@ -3617,7 +3617,7 @@
     </row>
     <row r="19" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>100123456</v>
+        <v>100000958</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>179</v>
@@ -3715,7 +3715,7 @@
     </row>
     <row r="20" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>100123456</v>
+        <v>100000959</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>173</v>
@@ -3813,7 +3813,7 @@
     </row>
     <row r="21" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>100123456</v>
+        <v>100000960</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>130</v>
@@ -3911,7 +3911,7 @@
     </row>
     <row r="22" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>100123456</v>
+        <v>100000961</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>153</v>
@@ -4009,7 +4009,7 @@
     </row>
     <row r="23" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>100123456</v>
+        <v>100000962</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>190</v>
@@ -4107,7 +4107,7 @@
     </row>
     <row r="24" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>100123456</v>
+        <v>100000963</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>193</v>
@@ -4205,7 +4205,7 @@
     </row>
     <row r="25" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>100123456</v>
+        <v>100000964</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>195</v>
@@ -4303,7 +4303,7 @@
     </row>
     <row r="26" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>100123456</v>
+        <v>100000965</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>147</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="27" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>100123456</v>
+        <v>100000966</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>147</v>
@@ -4499,7 +4499,7 @@
     </row>
     <row r="28" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>100123456</v>
+        <v>100000967</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>201</v>
@@ -4597,7 +4597,7 @@
     </row>
     <row r="29" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>100123456</v>
+        <v>100000968</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>192</v>
@@ -4695,7 +4695,7 @@
     </row>
     <row r="30" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>100123456</v>
+        <v>100000969</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>130</v>
@@ -4793,7 +4793,7 @@
     </row>
     <row r="31" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>100123456</v>
+        <v>100000970</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>191</v>
@@ -4891,7 +4891,7 @@
     </row>
     <row r="32" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>100123456</v>
+        <v>100000971</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>209</v>
@@ -4989,7 +4989,7 @@
     </row>
     <row r="33" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>100123456</v>
+        <v>100000972</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>134</v>
@@ -5087,7 +5087,7 @@
     </row>
     <row r="34" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>100123456</v>
+        <v>100000973</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>186</v>
@@ -5185,7 +5185,7 @@
     </row>
     <row r="35" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>100123456</v>
+        <v>100000974</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>135</v>
@@ -5283,7 +5283,7 @@
     </row>
     <row r="36" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>100123456</v>
+        <v>100000975</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>130</v>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="37" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>100123456</v>
+        <v>100000976</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>218</v>
@@ -5479,7 +5479,7 @@
     </row>
     <row r="38" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>100123456</v>
+        <v>100000977</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>221</v>
@@ -5577,7 +5577,7 @@
     </row>
     <row r="39" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>100123456</v>
+        <v>100000978</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>212</v>
@@ -5675,7 +5675,7 @@
     </row>
     <row r="40" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>100123456</v>
+        <v>100000979</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>155</v>
@@ -5773,7 +5773,7 @@
     </row>
     <row r="41" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>100123456</v>
+        <v>100000980</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>225</v>
@@ -5871,7 +5871,7 @@
     </row>
     <row r="42" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>100123456</v>
+        <v>100000981</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>163</v>
@@ -5969,7 +5969,7 @@
     </row>
     <row r="43" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>100123456</v>
+        <v>100000982</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>147</v>
@@ -6067,7 +6067,7 @@
     </row>
     <row r="44" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>100123456</v>
+        <v>100000983</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>230</v>
@@ -6165,7 +6165,7 @@
     </row>
     <row r="45" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>100123456</v>
+        <v>100000984</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>167</v>
@@ -6263,7 +6263,7 @@
     </row>
     <row r="46" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>100123456</v>
+        <v>100000985</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>233</v>
@@ -6361,7 +6361,7 @@
     </row>
     <row r="47" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>100123456</v>
+        <v>100000986</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>150</v>
@@ -6459,7 +6459,7 @@
     </row>
     <row r="48" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>100123456</v>
+        <v>100000987</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>235</v>
@@ -6557,7 +6557,7 @@
     </row>
     <row r="49" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>100123456</v>
+        <v>100000988</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>236</v>
@@ -6655,7 +6655,7 @@
     </row>
     <row r="50" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>100123456</v>
+        <v>100000989</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>144</v>
@@ -6753,7 +6753,7 @@
     </row>
     <row r="51" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>100123456</v>
+        <v>100000990</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>156</v>
@@ -6851,7 +6851,7 @@
     </row>
     <row r="52" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>100123456</v>
+        <v>100000991</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>240</v>
@@ -6949,7 +6949,7 @@
     </row>
     <row r="53" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>100123456</v>
+        <v>100000992</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>141</v>
@@ -7047,7 +7047,7 @@
     </row>
     <row r="54" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>100123456</v>
+        <v>100000993</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>242</v>
@@ -7145,7 +7145,7 @@
     </row>
     <row r="55" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>100123456</v>
+        <v>100000994</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>119</v>
@@ -7243,7 +7243,7 @@
     </row>
     <row r="56" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>100123456</v>
+        <v>100000995</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>174</v>
@@ -7341,7 +7341,7 @@
     </row>
     <row r="57" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>100123456</v>
+        <v>100000996</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>248</v>
@@ -7439,7 +7439,7 @@
     </row>
     <row r="58" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>100123456</v>
+        <v>100000997</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>250</v>
@@ -7537,7 +7537,7 @@
     </row>
     <row r="59" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>100123456</v>
+        <v>100000998</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>150</v>
@@ -7635,7 +7635,7 @@
     </row>
     <row r="60" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>100123456</v>
+        <v>100000999</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>252</v>
@@ -7733,7 +7733,7 @@
     </row>
     <row r="61" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>100123456</v>
+        <v>100001000</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>254</v>
@@ -7831,7 +7831,7 @@
     </row>
     <row r="62" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>100123456</v>
+        <v>100001001</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>124</v>
@@ -7929,7 +7929,7 @@
     </row>
     <row r="63" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>100123456</v>
+        <v>100001002</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>171</v>
@@ -8027,7 +8027,7 @@
     </row>
     <row r="64" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>100123456</v>
+        <v>100001003</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>196</v>
@@ -8125,7 +8125,7 @@
     </row>
     <row r="65" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>100123456</v>
+        <v>100001004</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>115</v>
@@ -8223,7 +8223,7 @@
     </row>
     <row r="66" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>100123456</v>
+        <v>100001005</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>161</v>
@@ -8321,7 +8321,7 @@
     </row>
     <row r="67" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>100123456</v>
+        <v>100001006</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>261</v>
@@ -8419,7 +8419,7 @@
     </row>
     <row r="68" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>100123456</v>
+        <v>100001007</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>151</v>
@@ -8517,7 +8517,7 @@
     </row>
     <row r="69" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>100123456</v>
+        <v>100001008</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>251</v>
@@ -8615,7 +8615,7 @@
     </row>
     <row r="70" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>100123456</v>
+        <v>100001009</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>126</v>
@@ -8713,7 +8713,7 @@
     </row>
     <row r="71" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>100123456</v>
+        <v>100001010</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>265</v>
@@ -8811,7 +8811,7 @@
     </row>
     <row r="72" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>100123456</v>
+        <v>100001011</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>213</v>
@@ -8909,7 +8909,7 @@
     </row>
     <row r="73" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>100123456</v>
+        <v>100001012</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>267</v>
@@ -9007,7 +9007,7 @@
     </row>
     <row r="74" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>100123456</v>
+        <v>100001013</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>269</v>
@@ -9105,7 +9105,7 @@
     </row>
     <row r="75" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>100123456</v>
+        <v>100001014</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>271</v>
@@ -9203,7 +9203,7 @@
     </row>
     <row r="76" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>100123456</v>
+        <v>100001015</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>273</v>
@@ -9301,7 +9301,7 @@
     </row>
     <row r="77" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>100123456</v>
+        <v>100001016</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>246</v>
@@ -9399,7 +9399,7 @@
     </row>
     <row r="78" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>100123456</v>
+        <v>100001017</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>276</v>
@@ -9497,7 +9497,7 @@
     </row>
     <row r="79" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>100123456</v>
+        <v>100001018</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>279</v>
@@ -9595,7 +9595,7 @@
     </row>
     <row r="80" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>100123456</v>
+        <v>100001019</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>139</v>
@@ -9693,7 +9693,7 @@
     </row>
     <row r="81" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>100123456</v>
+        <v>100001020</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>216</v>
@@ -9791,7 +9791,7 @@
     </row>
     <row r="82" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>100123456</v>
+        <v>100001021</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>282</v>
@@ -9889,7 +9889,7 @@
     </row>
     <row r="83" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>100123456</v>
+        <v>100001022</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>283</v>
@@ -9987,7 +9987,7 @@
     </row>
     <row r="84" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>100123456</v>
+        <v>100001023</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>168</v>
@@ -10085,7 +10085,7 @@
     </row>
     <row r="85" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>100123456</v>
+        <v>100001024</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>138</v>
@@ -10183,7 +10183,7 @@
     </row>
     <row r="86" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>100123456</v>
+        <v>100001025</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>133</v>
@@ -10281,7 +10281,7 @@
     </row>
     <row r="87" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>100123456</v>
+        <v>100001026</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>177</v>
@@ -10379,7 +10379,7 @@
     </row>
     <row r="88" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>100123456</v>
+        <v>100001027</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>286</v>
@@ -10477,7 +10477,7 @@
     </row>
     <row r="89" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>100123456</v>
+        <v>100001028</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>288</v>
@@ -10575,7 +10575,7 @@
     </row>
     <row r="90" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>100123456</v>
+        <v>100001029</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>290</v>
@@ -10673,7 +10673,7 @@
     </row>
     <row r="91" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>100123456</v>
+        <v>100001030</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>292</v>
@@ -10771,7 +10771,7 @@
     </row>
     <row r="92" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>100123456</v>
+        <v>100001031</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>294</v>
@@ -10869,7 +10869,7 @@
     </row>
     <row r="93" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>100123456</v>
+        <v>100001032</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>296</v>
@@ -10967,7 +10967,7 @@
     </row>
     <row r="94" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>100123456</v>
+        <v>100001033</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>232</v>
@@ -11065,7 +11065,7 @@
     </row>
     <row r="95" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>100123456</v>
+        <v>100001034</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>203</v>
@@ -11163,7 +11163,7 @@
     </row>
     <row r="96" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>100123456</v>
+        <v>100001035</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>160</v>
@@ -11261,7 +11261,7 @@
     </row>
     <row r="97" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>100123456</v>
+        <v>100001036</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>217</v>
@@ -11359,7 +11359,7 @@
     </row>
     <row r="98" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>100123456</v>
+        <v>100001037</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>301</v>
@@ -11457,7 +11457,7 @@
     </row>
     <row r="99" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <v>100123456</v>
+        <v>100001038</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>244</v>
@@ -11555,7 +11555,7 @@
     </row>
     <row r="100" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>100123456</v>
+        <v>100001039</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>178</v>
@@ -11653,7 +11653,7 @@
     </row>
     <row r="101" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>100123456</v>
+        <v>100001040</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>184</v>
@@ -11751,7 +11751,7 @@
     </row>
     <row r="102" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>100123456</v>
+        <v>100001041</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>305</v>
@@ -11849,7 +11849,7 @@
     </row>
     <row r="103" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>100123456</v>
+        <v>100001042</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>306</v>
@@ -11947,7 +11947,7 @@
     </row>
     <row r="104" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>100123456</v>
+        <v>100001043</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>206</v>
@@ -12045,7 +12045,7 @@
     </row>
     <row r="105" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>100123456</v>
+        <v>100001044</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>153</v>
@@ -12143,7 +12143,7 @@
     </row>
     <row r="106" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>100123456</v>
+        <v>100001045</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>208</v>
@@ -12241,7 +12241,7 @@
     </row>
     <row r="107" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>100123456</v>
+        <v>100001046</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>115</v>
@@ -12339,7 +12339,7 @@
     </row>
     <row r="108" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>100123456</v>
+        <v>100001047</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>278</v>
@@ -12437,7 +12437,7 @@
     </row>
     <row r="109" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>100123456</v>
+        <v>100001048</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>186</v>
@@ -12535,7 +12535,7 @@
     </row>
     <row r="110" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>100123456</v>
+        <v>100001049</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>177</v>
@@ -12651,15 +12651,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046EA511BBCB59E42A88A619BFC75661B" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="280e44903c962187b208735be74fa2e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48c5b5cd9b8d25ff6dd15848836f4270" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -12791,6 +12782,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -12801,14 +12801,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1782932A-B736-4F6B-91B2-C27EF01688B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE0B7BE3-D1EB-49DA-AABC-5B30932E3CDA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12822,6 +12814,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1782932A-B736-4F6B-91B2-C27EF01688B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>